<commit_message>
et: sch/stm may 2021 - updates
</commit_message>
<xml_diff>
--- a/SCH-STH/Baseline Mapping/Ethiopia/eth_sch_sth_remaping_1_school_202105.xlsx
+++ b/SCH-STH/Baseline Mapping/Ethiopia/eth_sch_sth_remaping_1_school_202105.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\SCH-STH\Baseline Mapping\Ethiopia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C8448C-9A94-41C7-9A44-B8CD3EDB690B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73377D4D-4CFC-40CE-AF52-A035BA7E2460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="3" r:id="rId2"/>
     <sheet name="settings" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateCount="1000" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1975" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1978" uniqueCount="713">
   <si>
     <t>label</t>
   </si>
@@ -2150,15 +2150,9 @@
     <t>.&gt;=1 and .&lt;=8 and .&gt;=${c_lowestGrade}</t>
   </si>
   <si>
-    <t>1. Ethiopia - Reassessment Form School</t>
-  </si>
-  <si>
     <t>c_school_code</t>
   </si>
   <si>
-    <t>eth_sch_sth_remaping_1_school_202105</t>
-  </si>
-  <si>
     <t>. &gt; 99 and . &lt; 1000</t>
   </si>
   <si>
@@ -2169,6 +2163,21 @@
   </si>
   <si>
     <t>c_school_code_other</t>
+  </si>
+  <si>
+    <t>regex(.,'^[0-9]{10}$')</t>
+  </si>
+  <si>
+    <t>The phone number is restricted to 10 digits</t>
+  </si>
+  <si>
+    <t>eth_sch_sth_remaping_1_school_202105_V2</t>
+  </si>
+  <si>
+    <t>202105_V2</t>
+  </si>
+  <si>
+    <t>1. Ethiopia - Reassessment Form School V2</t>
   </si>
 </sst>
 </file>
@@ -3428,32 +3437,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="43.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.87890625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5859375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.41015625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="43.29296875" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
     <col min="7" max="7" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="14.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.29296875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5859375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.29296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1171875" style="1"/>
+    <col min="13" max="13" width="14.703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="15" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="16384" width="9.1171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
@@ -3497,7 +3506,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -3518,7 +3527,7 @@
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="11"/>
@@ -3533,7 +3542,7 @@
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -3544,7 +3553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -3567,7 +3576,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>95</v>
       </c>
@@ -3581,7 +3590,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>98</v>
       </c>
@@ -3598,7 +3607,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>99</v>
       </c>
@@ -3618,7 +3627,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -3635,7 +3644,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>100</v>
       </c>
@@ -3649,7 +3658,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -3666,21 +3675,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>696</v>
       </c>
       <c r="F14" s="41" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="H14" s="41" t="s">
         <v>692</v>
@@ -3689,12 +3698,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="C15" s="41" t="s">
         <v>102</v>
@@ -3706,21 +3715,21 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="41" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="41" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="C16" s="41" t="s">
         <v>696</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="H16" s="41" t="s">
         <v>695</v>
@@ -3729,7 +3738,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -3743,9 +3752,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="37" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A18" s="37" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>110</v>
@@ -3753,11 +3762,17 @@
       <c r="C18" s="37" t="s">
         <v>13</v>
       </c>
+      <c r="F18" s="37" t="s">
+        <v>708</v>
+      </c>
+      <c r="G18" s="37" t="s">
+        <v>709</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>115</v>
       </c>
@@ -3771,7 +3786,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>118</v>
       </c>
@@ -3791,7 +3806,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -3814,7 +3829,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -3828,7 +3843,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -3842,7 +3857,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -3856,7 +3871,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -3870,7 +3885,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>6</v>
       </c>
@@ -3884,7 +3899,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>6</v>
       </c>
@@ -3898,7 +3913,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
@@ -3912,7 +3927,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
@@ -3926,7 +3941,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -3946,7 +3961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>6</v>
       </c>
@@ -3960,7 +3975,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>6</v>
       </c>
@@ -3974,7 +3989,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -3988,7 +4003,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
@@ -4002,7 +4017,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>6</v>
       </c>
@@ -4016,7 +4031,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
@@ -4030,7 +4045,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>6</v>
       </c>
@@ -4044,7 +4059,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>6</v>
       </c>
@@ -4058,7 +4073,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -4078,7 +4093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="43" x14ac:dyDescent="0.5">
       <c r="A40" s="7" t="s">
         <v>2</v>
       </c>
@@ -4093,7 +4108,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>141</v>
       </c>
@@ -4107,7 +4122,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>153</v>
       </c>
@@ -4121,7 +4136,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
         <v>153</v>
       </c>
@@ -4135,7 +4150,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>158</v>
       </c>
@@ -4149,7 +4164,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>153</v>
       </c>
@@ -4163,7 +4178,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>153</v>
       </c>
@@ -4177,7 +4192,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>6</v>
       </c>
@@ -4191,7 +4206,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>153</v>
       </c>
@@ -4205,7 +4220,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
         <v>172</v>
       </c>
@@ -4222,7 +4237,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -4239,7 +4254,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="43" x14ac:dyDescent="0.5">
       <c r="A51" s="7" t="s">
         <v>2</v>
       </c>
@@ -4253,7 +4268,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
     </row>
-    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A52" s="1" t="s">
         <v>178</v>
       </c>
@@ -4267,7 +4282,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="43" x14ac:dyDescent="0.5">
       <c r="A53" s="1" t="s">
         <v>6</v>
       </c>
@@ -4281,7 +4296,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A54" s="1" t="s">
         <v>153</v>
       </c>
@@ -4295,7 +4310,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A55" s="1" t="s">
         <v>194</v>
       </c>
@@ -4309,7 +4324,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A56" s="1" t="s">
         <v>153</v>
       </c>
@@ -4323,7 +4338,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A57" s="1" t="s">
         <v>153</v>
       </c>
@@ -4337,7 +4352,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A58" s="1" t="s">
         <v>200</v>
       </c>
@@ -4351,7 +4366,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A59" s="1" t="s">
         <v>213</v>
       </c>
@@ -4365,7 +4380,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A60" s="1" t="s">
         <v>153</v>
       </c>
@@ -4379,7 +4394,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A61" s="1" t="s">
         <v>153</v>
       </c>
@@ -4393,7 +4408,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A62" s="1" t="s">
         <v>221</v>
       </c>
@@ -4407,7 +4422,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A63" s="1" t="s">
         <v>227</v>
       </c>
@@ -4421,7 +4436,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A64" s="1" t="s">
         <v>153</v>
       </c>
@@ -4435,7 +4450,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A65" s="1" t="s">
         <v>234</v>
       </c>
@@ -4449,7 +4464,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A66" s="1" t="s">
         <v>153</v>
       </c>
@@ -4463,10 +4478,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.5">
       <c r="C67" s="6"/>
     </row>
-    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="43" x14ac:dyDescent="0.5">
       <c r="A68" s="7" t="s">
         <v>2</v>
       </c>
@@ -4480,7 +4495,7 @@
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A69" s="1" t="s">
         <v>153</v>
       </c>
@@ -4494,7 +4509,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A70" s="1" t="s">
         <v>241</v>
       </c>
@@ -4511,7 +4526,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
@@ -4528,7 +4543,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A72" s="1" t="s">
         <v>153</v>
       </c>
@@ -4545,7 +4560,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A73" s="1" t="s">
         <v>256</v>
       </c>
@@ -4562,7 +4577,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
@@ -4580,7 +4595,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
@@ -4597,7 +4612,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A76" s="1" t="s">
         <v>264</v>
       </c>
@@ -4611,7 +4626,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A77" s="1" t="s">
         <v>270</v>
       </c>
@@ -4625,7 +4640,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A78" s="1" t="s">
         <v>276</v>
       </c>
@@ -4639,7 +4654,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A80" s="1" t="s">
         <v>324</v>
       </c>
@@ -4650,7 +4665,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" s="1" t="s">
         <v>327</v>
       </c>
@@ -4962,16 +4977,16 @@
       <selection pane="bottomRight" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="28" style="14" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="58.41015625" style="14" customWidth="1"/>
     <col min="3" max="3" width="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.41015625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="29" t="s">
         <v>111</v>
       </c>
@@ -4988,7 +5003,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
@@ -4999,7 +5014,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
@@ -5010,7 +5025,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="15" t="s">
         <v>5</v>
       </c>
@@ -5021,7 +5036,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5047,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="15" t="s">
         <v>5</v>
       </c>
@@ -5043,7 +5058,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
@@ -5054,7 +5069,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
@@ -5065,7 +5080,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15" t="s">
         <v>5</v>
       </c>
@@ -5076,12 +5091,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="21"/>
       <c r="B11" s="38"/>
       <c r="C11" s="39"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" s="15" t="s">
         <v>143</v>
       </c>
@@ -5092,7 +5107,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="15" t="s">
         <v>143</v>
       </c>
@@ -5103,7 +5118,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="15" t="s">
         <v>143</v>
       </c>
@@ -5114,7 +5129,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="15" t="s">
         <v>143</v>
       </c>
@@ -5125,7 +5140,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="15" t="s">
         <v>143</v>
       </c>
@@ -5136,7 +5151,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="15" t="s">
         <v>143</v>
       </c>
@@ -5147,7 +5162,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" s="15" t="s">
         <v>143</v>
       </c>
@@ -5158,7 +5173,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" s="15" t="s">
         <v>143</v>
       </c>
@@ -5169,12 +5184,12 @@
         <v>289</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="21"/>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="24" t="s">
         <v>154</v>
       </c>
@@ -5185,7 +5200,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="24" t="s">
         <v>154</v>
       </c>
@@ -5196,12 +5211,12 @@
         <v>291</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="26"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" s="15" t="s">
         <v>160</v>
       </c>
@@ -5212,7 +5227,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" s="15" t="s">
         <v>160</v>
       </c>
@@ -5223,7 +5238,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" s="15" t="s">
         <v>160</v>
       </c>
@@ -5234,11 +5249,11 @@
         <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" s="21"/>
       <c r="B27" s="22"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" s="15" t="s">
         <v>173</v>
       </c>
@@ -5249,7 +5264,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" s="15" t="s">
         <v>173</v>
       </c>
@@ -5260,7 +5275,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" s="15" t="s">
         <v>173</v>
       </c>
@@ -5271,7 +5286,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" s="15" t="s">
         <v>173</v>
       </c>
@@ -5282,7 +5297,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" s="15" t="s">
         <v>173</v>
       </c>
@@ -5293,7 +5308,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" s="15" t="s">
         <v>173</v>
       </c>
@@ -5304,16 +5319,16 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" s="18"/>
       <c r="B34" s="19"/>
       <c r="C34" s="20"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" s="21"/>
       <c r="B35" s="22"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" s="15" t="s">
         <v>179</v>
       </c>
@@ -5324,7 +5339,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" s="15" t="s">
         <v>179</v>
       </c>
@@ -5335,7 +5350,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" s="15" t="s">
         <v>179</v>
       </c>
@@ -5346,7 +5361,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" s="15" t="s">
         <v>179</v>
       </c>
@@ -5357,7 +5372,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" s="15" t="s">
         <v>179</v>
       </c>
@@ -5368,7 +5383,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" s="15" t="s">
         <v>179</v>
       </c>
@@ -5379,7 +5394,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" s="15" t="s">
         <v>179</v>
       </c>
@@ -5390,11 +5405,11 @@
         <v>186</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" s="21"/>
       <c r="B43" s="22"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" s="13" t="s">
         <v>195</v>
       </c>
@@ -5405,7 +5420,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" s="13" t="s">
         <v>195</v>
       </c>
@@ -5416,7 +5431,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" s="13" t="s">
         <v>195</v>
       </c>
@@ -5427,11 +5442,11 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" s="21"/>
       <c r="B47" s="22"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" s="15" t="s">
         <v>201</v>
       </c>
@@ -5442,7 +5457,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A49" s="15" t="s">
         <v>201</v>
       </c>
@@ -5453,7 +5468,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A50" s="15" t="s">
         <v>201</v>
       </c>
@@ -5464,7 +5479,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A51" s="15" t="s">
         <v>201</v>
       </c>
@@ -5475,11 +5490,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A52" s="21"/>
       <c r="B52" s="22"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A53" s="15" t="s">
         <v>214</v>
       </c>
@@ -5490,7 +5505,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A54" s="15" t="s">
         <v>214</v>
       </c>
@@ -5501,7 +5516,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A55" s="15" t="s">
         <v>214</v>
       </c>
@@ -5512,11 +5527,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A56" s="21"/>
       <c r="B56" s="22"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A57" s="15" t="s">
         <v>222</v>
       </c>
@@ -5527,7 +5542,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A58" s="15" t="s">
         <v>222</v>
       </c>
@@ -5538,7 +5553,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A59" s="15" t="s">
         <v>222</v>
       </c>
@@ -5549,11 +5564,11 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A60" s="21"/>
       <c r="B60" s="22"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A61" s="15" t="s">
         <v>228</v>
       </c>
@@ -5564,7 +5579,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A62" s="15" t="s">
         <v>228</v>
       </c>
@@ -5575,7 +5590,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A63" s="15" t="s">
         <v>228</v>
       </c>
@@ -5586,11 +5601,11 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A64" s="21"/>
       <c r="B64" s="22"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A65" s="15" t="s">
         <v>235</v>
       </c>
@@ -5601,7 +5616,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A66" s="15" t="s">
         <v>235</v>
       </c>
@@ -5612,7 +5627,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A67" s="15" t="s">
         <v>235</v>
       </c>
@@ -5623,11 +5638,11 @@
         <v>238</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A68" s="21"/>
       <c r="B68" s="22"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A69" s="15" t="s">
         <v>242</v>
       </c>
@@ -5638,7 +5653,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A70" s="15" t="s">
         <v>242</v>
       </c>
@@ -5649,7 +5664,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A71" s="15" t="s">
         <v>242</v>
       </c>
@@ -5660,7 +5675,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A72" s="15" t="s">
         <v>242</v>
       </c>
@@ -5671,11 +5686,11 @@
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A73" s="32"/>
       <c r="B73" s="33"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A74" s="15" t="s">
         <v>257</v>
       </c>
@@ -5686,7 +5701,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A75" s="15" t="s">
         <v>257</v>
       </c>
@@ -5697,7 +5712,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A76" s="15" t="s">
         <v>257</v>
       </c>
@@ -5708,7 +5723,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A77" s="15" t="s">
         <v>257</v>
       </c>
@@ -5719,7 +5734,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A78" s="15" t="s">
         <v>257</v>
       </c>
@@ -5730,7 +5745,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A79" s="15" t="s">
         <v>257</v>
       </c>
@@ -5741,11 +5756,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A80" s="21"/>
       <c r="B80" s="22"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A81" s="15" t="s">
         <v>268</v>
       </c>
@@ -5756,7 +5771,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A82" s="15" t="s">
         <v>268</v>
       </c>
@@ -5767,7 +5782,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A83" s="15" t="s">
         <v>268</v>
       </c>
@@ -5778,7 +5793,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A84" s="15" t="s">
         <v>268</v>
       </c>
@@ -5789,11 +5804,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A85" s="21"/>
       <c r="B85" s="22"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A86" s="15" t="s">
         <v>272</v>
       </c>
@@ -5804,7 +5819,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A87" s="15" t="s">
         <v>272</v>
       </c>
@@ -5815,7 +5830,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A88" s="15" t="s">
         <v>272</v>
       </c>
@@ -5826,11 +5841,11 @@
         <v>275</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A89" s="21"/>
       <c r="B89" s="22"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A90" s="15" t="s">
         <v>278</v>
       </c>
@@ -5841,7 +5856,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A91" s="15" t="s">
         <v>278</v>
       </c>
@@ -5852,7 +5867,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A92" s="15" t="s">
         <v>278</v>
       </c>
@@ -5863,7 +5878,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A93" s="15" t="s">
         <v>278</v>
       </c>
@@ -5874,7 +5889,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A97" s="14" t="s">
         <v>112</v>
       </c>
@@ -5887,7 +5902,7 @@
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A98" s="14" t="s">
         <v>112</v>
       </c>
@@ -5900,7 +5915,7 @@
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A99" s="14" t="s">
         <v>112</v>
       </c>
@@ -5913,7 +5928,7 @@
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A100" s="14" t="s">
         <v>112</v>
       </c>
@@ -5926,12 +5941,12 @@
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C101" s="14"/>
       <c r="D101" s="14"/>
       <c r="E101" s="14"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A102" s="14" t="s">
         <v>113</v>
       </c>
@@ -5946,7 +5961,7 @@
       </c>
       <c r="E102" s="14"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A103" s="14" t="s">
         <v>113</v>
       </c>
@@ -5961,7 +5976,7 @@
       </c>
       <c r="E103" s="14"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A104" s="14" t="s">
         <v>113</v>
       </c>
@@ -5976,7 +5991,7 @@
       </c>
       <c r="E104" s="14"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A105" s="14" t="s">
         <v>113</v>
       </c>
@@ -5991,7 +6006,7 @@
       </c>
       <c r="E105" s="14"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A106" s="14" t="s">
         <v>113</v>
       </c>
@@ -6006,7 +6021,7 @@
       </c>
       <c r="E106" s="14"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A107" s="14" t="s">
         <v>113</v>
       </c>
@@ -6021,7 +6036,7 @@
       </c>
       <c r="E107" s="14"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A108" s="14" t="s">
         <v>113</v>
       </c>
@@ -6036,7 +6051,7 @@
       </c>
       <c r="E108" s="14"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A109" s="14" t="s">
         <v>113</v>
       </c>
@@ -6051,7 +6066,7 @@
       </c>
       <c r="E109" s="14"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A110" s="14" t="s">
         <v>113</v>
       </c>
@@ -6066,7 +6081,7 @@
       </c>
       <c r="E110" s="14"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A111" s="14" t="s">
         <v>113</v>
       </c>
@@ -6081,7 +6096,7 @@
       </c>
       <c r="E111" s="14"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A112" s="14" t="s">
         <v>113</v>
       </c>
@@ -6096,7 +6111,7 @@
       </c>
       <c r="E112" s="14"/>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A113" s="14" t="s">
         <v>113</v>
       </c>
@@ -6111,7 +6126,7 @@
       </c>
       <c r="E113" s="14"/>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A114" s="14" t="s">
         <v>113</v>
       </c>
@@ -6126,7 +6141,7 @@
       </c>
       <c r="E114" s="14"/>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A115" s="14" t="s">
         <v>113</v>
       </c>
@@ -6141,7 +6156,7 @@
       </c>
       <c r="E115" s="14"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A116" s="14" t="s">
         <v>113</v>
       </c>
@@ -6156,7 +6171,7 @@
       </c>
       <c r="E116" s="14"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A117" s="14" t="s">
         <v>113</v>
       </c>
@@ -6171,7 +6186,7 @@
       </c>
       <c r="E117" s="14"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A118" s="14" t="s">
         <v>113</v>
       </c>
@@ -6186,7 +6201,7 @@
       </c>
       <c r="E118" s="14"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A119" s="14" t="s">
         <v>113</v>
       </c>
@@ -6201,7 +6216,7 @@
       </c>
       <c r="E119" s="14"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A120" s="14" t="s">
         <v>113</v>
       </c>
@@ -6216,7 +6231,7 @@
       </c>
       <c r="E120" s="14"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A121" s="14" t="s">
         <v>113</v>
       </c>
@@ -6231,7 +6246,7 @@
       </c>
       <c r="E121" s="14"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A122" s="14" t="s">
         <v>113</v>
       </c>
@@ -6246,7 +6261,7 @@
       </c>
       <c r="E122" s="14"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A123" s="14" t="s">
         <v>113</v>
       </c>
@@ -6261,7 +6276,7 @@
       </c>
       <c r="E123" s="14"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A124" s="14" t="s">
         <v>113</v>
       </c>
@@ -6276,7 +6291,7 @@
       </c>
       <c r="E124" s="14"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A125" s="14" t="s">
         <v>113</v>
       </c>
@@ -6291,7 +6306,7 @@
       </c>
       <c r="E125" s="14"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A126" s="14" t="s">
         <v>113</v>
       </c>
@@ -6306,7 +6321,7 @@
       </c>
       <c r="E126" s="14"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A127" s="14" t="s">
         <v>113</v>
       </c>
@@ -6321,7 +6336,7 @@
       </c>
       <c r="E127" s="14"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A128" s="14" t="s">
         <v>113</v>
       </c>
@@ -6336,7 +6351,7 @@
       </c>
       <c r="E128" s="14"/>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A129" s="14" t="s">
         <v>113</v>
       </c>
@@ -6351,7 +6366,7 @@
       </c>
       <c r="E129" s="14"/>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A130" s="14" t="s">
         <v>113</v>
       </c>
@@ -6366,7 +6381,7 @@
       </c>
       <c r="E130" s="14"/>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A131" s="14" t="s">
         <v>113</v>
       </c>
@@ -6381,7 +6396,7 @@
       </c>
       <c r="E131" s="14"/>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A132" s="14" t="s">
         <v>113</v>
       </c>
@@ -6396,7 +6411,7 @@
       </c>
       <c r="E132" s="14"/>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A133" s="14" t="s">
         <v>113</v>
       </c>
@@ -6411,7 +6426,7 @@
       </c>
       <c r="E133" s="14"/>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A134" s="14" t="s">
         <v>113</v>
       </c>
@@ -6426,7 +6441,7 @@
       </c>
       <c r="E134" s="14"/>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A135" s="14" t="s">
         <v>113</v>
       </c>
@@ -6441,7 +6456,7 @@
       </c>
       <c r="E135" s="14"/>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A136" s="14" t="s">
         <v>113</v>
       </c>
@@ -6456,7 +6471,7 @@
       </c>
       <c r="E136" s="14"/>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A137" s="14" t="s">
         <v>113</v>
       </c>
@@ -6471,7 +6486,7 @@
       </c>
       <c r="E137" s="14"/>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A138" s="14" t="s">
         <v>113</v>
       </c>
@@ -6486,7 +6501,7 @@
       </c>
       <c r="E138" s="14"/>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A139" s="14" t="s">
         <v>113</v>
       </c>
@@ -6501,7 +6516,7 @@
       </c>
       <c r="E139" s="14"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A140" s="14" t="s">
         <v>113</v>
       </c>
@@ -6516,7 +6531,7 @@
       </c>
       <c r="E140" s="14"/>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A141" s="14" t="s">
         <v>113</v>
       </c>
@@ -6531,7 +6546,7 @@
       </c>
       <c r="E141" s="14"/>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A142" s="14" t="s">
         <v>113</v>
       </c>
@@ -6546,7 +6561,7 @@
       </c>
       <c r="E142" s="14"/>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A143" s="14" t="s">
         <v>113</v>
       </c>
@@ -6561,7 +6576,7 @@
       </c>
       <c r="E143" s="14"/>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A144" s="14" t="s">
         <v>113</v>
       </c>
@@ -6576,7 +6591,7 @@
       </c>
       <c r="E144" s="14"/>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A145" s="14" t="s">
         <v>113</v>
       </c>
@@ -6591,7 +6606,7 @@
       </c>
       <c r="E145" s="14"/>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A146" s="14" t="s">
         <v>113</v>
       </c>
@@ -6606,7 +6621,7 @@
       </c>
       <c r="E146" s="14"/>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A147" s="14" t="s">
         <v>113</v>
       </c>
@@ -6621,7 +6636,7 @@
       </c>
       <c r="E147" s="14"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A148" s="14" t="s">
         <v>113</v>
       </c>
@@ -6636,7 +6651,7 @@
       </c>
       <c r="E148" s="14"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A149" s="14" t="s">
         <v>113</v>
       </c>
@@ -6651,7 +6666,7 @@
       </c>
       <c r="E149" s="14"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A150" s="14" t="s">
         <v>113</v>
       </c>
@@ -6666,7 +6681,7 @@
       </c>
       <c r="E150" s="14"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A151" s="14" t="s">
         <v>113</v>
       </c>
@@ -6681,7 +6696,7 @@
       </c>
       <c r="E151" s="14"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A152" s="14" t="s">
         <v>113</v>
       </c>
@@ -6696,7 +6711,7 @@
       </c>
       <c r="E152" s="14"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A153" s="14" t="s">
         <v>113</v>
       </c>
@@ -6711,7 +6726,7 @@
       </c>
       <c r="E153" s="14"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A154" s="14" t="s">
         <v>113</v>
       </c>
@@ -6726,7 +6741,7 @@
       </c>
       <c r="E154" s="14"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A155" s="14" t="s">
         <v>113</v>
       </c>
@@ -6741,7 +6756,7 @@
       </c>
       <c r="E155" s="14"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A156" s="14" t="s">
         <v>113</v>
       </c>
@@ -6756,7 +6771,7 @@
       </c>
       <c r="E156" s="14"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A157" s="14" t="s">
         <v>113</v>
       </c>
@@ -6771,7 +6786,7 @@
       </c>
       <c r="E157" s="14"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A158" s="14" t="s">
         <v>113</v>
       </c>
@@ -6786,7 +6801,7 @@
       </c>
       <c r="E158" s="14"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A159" s="14" t="s">
         <v>113</v>
       </c>
@@ -6801,7 +6816,7 @@
       </c>
       <c r="E159" s="14"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A160" s="14" t="s">
         <v>113</v>
       </c>
@@ -6816,7 +6831,7 @@
       </c>
       <c r="E160" s="14"/>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A161" s="14" t="s">
         <v>113</v>
       </c>
@@ -6831,7 +6846,7 @@
       </c>
       <c r="E161" s="14"/>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A162" s="14" t="s">
         <v>113</v>
       </c>
@@ -6846,7 +6861,7 @@
       </c>
       <c r="E162" s="14"/>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A163" s="14" t="s">
         <v>113</v>
       </c>
@@ -6861,7 +6876,7 @@
       </c>
       <c r="E163" s="14"/>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A164" s="14" t="s">
         <v>113</v>
       </c>
@@ -6876,7 +6891,7 @@
       </c>
       <c r="E164" s="14"/>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A165" s="14" t="s">
         <v>113</v>
       </c>
@@ -6891,7 +6906,7 @@
       </c>
       <c r="E165" s="14"/>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A166" s="14" t="s">
         <v>113</v>
       </c>
@@ -6906,7 +6921,7 @@
       </c>
       <c r="E166" s="14"/>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A167" s="14" t="s">
         <v>113</v>
       </c>
@@ -6921,7 +6936,7 @@
       </c>
       <c r="E167" s="14"/>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A168" s="14" t="s">
         <v>113</v>
       </c>
@@ -6936,7 +6951,7 @@
       </c>
       <c r="E168" s="14"/>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A169" s="14" t="s">
         <v>113</v>
       </c>
@@ -6951,7 +6966,7 @@
       </c>
       <c r="E169" s="14"/>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A170" s="14" t="s">
         <v>113</v>
       </c>
@@ -6966,7 +6981,7 @@
       </c>
       <c r="E170" s="14"/>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A171" s="14" t="s">
         <v>113</v>
       </c>
@@ -6981,7 +6996,7 @@
       </c>
       <c r="E171" s="14"/>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A172" s="14" t="s">
         <v>113</v>
       </c>
@@ -6996,7 +7011,7 @@
       </c>
       <c r="E172" s="14"/>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A173" s="14" t="s">
         <v>113</v>
       </c>
@@ -7011,7 +7026,7 @@
       </c>
       <c r="E173" s="14"/>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A174" s="14" t="s">
         <v>113</v>
       </c>
@@ -7026,7 +7041,7 @@
       </c>
       <c r="E174" s="14"/>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A175" s="14" t="s">
         <v>113</v>
       </c>
@@ -7041,7 +7056,7 @@
       </c>
       <c r="E175" s="14"/>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A176" s="14" t="s">
         <v>113</v>
       </c>
@@ -7056,7 +7071,7 @@
       </c>
       <c r="E176" s="14"/>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A177" s="14" t="s">
         <v>113</v>
       </c>
@@ -7071,7 +7086,7 @@
       </c>
       <c r="E177" s="14"/>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A178" s="14" t="s">
         <v>113</v>
       </c>
@@ -7086,7 +7101,7 @@
       </c>
       <c r="E178" s="14"/>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A179" s="14" t="s">
         <v>113</v>
       </c>
@@ -7101,7 +7116,7 @@
       </c>
       <c r="E179" s="14"/>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A180" s="14" t="s">
         <v>113</v>
       </c>
@@ -7116,7 +7131,7 @@
       </c>
       <c r="E180" s="14"/>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A181" s="14" t="s">
         <v>113</v>
       </c>
@@ -7131,7 +7146,7 @@
       </c>
       <c r="E181" s="14"/>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A182" s="14" t="s">
         <v>113</v>
       </c>
@@ -7146,7 +7161,7 @@
       </c>
       <c r="E182" s="14"/>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A183" s="14" t="s">
         <v>113</v>
       </c>
@@ -7161,7 +7176,7 @@
       </c>
       <c r="E183" s="14"/>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A184" s="14" t="s">
         <v>113</v>
       </c>
@@ -7176,7 +7191,7 @@
       </c>
       <c r="E184" s="14"/>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A185" s="14" t="s">
         <v>113</v>
       </c>
@@ -7191,7 +7206,7 @@
       </c>
       <c r="E185" s="14"/>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A186" s="14" t="s">
         <v>113</v>
       </c>
@@ -7206,7 +7221,7 @@
       </c>
       <c r="E186" s="14"/>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A187" s="14" t="s">
         <v>113</v>
       </c>
@@ -7221,7 +7236,7 @@
       </c>
       <c r="E187" s="14"/>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A188" s="14" t="s">
         <v>113</v>
       </c>
@@ -7236,7 +7251,7 @@
       </c>
       <c r="E188" s="14"/>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A189" s="14" t="s">
         <v>113</v>
       </c>
@@ -7251,7 +7266,7 @@
       </c>
       <c r="E189" s="14"/>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A190" s="14" t="s">
         <v>113</v>
       </c>
@@ -7266,7 +7281,7 @@
       </c>
       <c r="E190" s="14"/>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A191" s="14" t="s">
         <v>113</v>
       </c>
@@ -7281,7 +7296,7 @@
       </c>
       <c r="E191" s="14"/>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A192" s="14" t="s">
         <v>113</v>
       </c>
@@ -7296,7 +7311,7 @@
       </c>
       <c r="E192" s="14"/>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A193" s="14" t="s">
         <v>113</v>
       </c>
@@ -7311,7 +7326,7 @@
       </c>
       <c r="E193" s="14"/>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A194" s="14" t="s">
         <v>113</v>
       </c>
@@ -7326,7 +7341,7 @@
       </c>
       <c r="E194" s="14"/>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A195" s="14" t="s">
         <v>113</v>
       </c>
@@ -7341,7 +7356,7 @@
       </c>
       <c r="E195" s="14"/>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A196" s="14" t="s">
         <v>113</v>
       </c>
@@ -7356,7 +7371,7 @@
       </c>
       <c r="E196" s="14"/>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A197" s="14" t="s">
         <v>113</v>
       </c>
@@ -7371,7 +7386,7 @@
       </c>
       <c r="E197" s="14"/>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A198" s="14" t="s">
         <v>113</v>
       </c>
@@ -7386,7 +7401,7 @@
       </c>
       <c r="E198" s="14"/>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A199" s="14" t="s">
         <v>113</v>
       </c>
@@ -7401,7 +7416,7 @@
       </c>
       <c r="E199" s="14"/>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A200" s="14" t="s">
         <v>113</v>
       </c>
@@ -7416,7 +7431,7 @@
       </c>
       <c r="E200" s="14"/>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A201" s="14" t="s">
         <v>113</v>
       </c>
@@ -7431,7 +7446,7 @@
       </c>
       <c r="E201" s="14"/>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A202" s="14" t="s">
         <v>113</v>
       </c>
@@ -7446,7 +7461,7 @@
       </c>
       <c r="E202" s="14"/>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A203" s="14" t="s">
         <v>113</v>
       </c>
@@ -7461,7 +7476,7 @@
       </c>
       <c r="E203" s="14"/>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A204" s="14" t="s">
         <v>113</v>
       </c>
@@ -7476,7 +7491,7 @@
       </c>
       <c r="E204" s="14"/>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A205" s="14" t="s">
         <v>113</v>
       </c>
@@ -7491,7 +7506,7 @@
       </c>
       <c r="E205" s="14"/>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A206" s="14" t="s">
         <v>113</v>
       </c>
@@ -7506,7 +7521,7 @@
       </c>
       <c r="E206" s="14"/>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A207" s="14" t="s">
         <v>113</v>
       </c>
@@ -7521,7 +7536,7 @@
       </c>
       <c r="E207" s="14"/>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A208" s="14" t="s">
         <v>113</v>
       </c>
@@ -7536,7 +7551,7 @@
       </c>
       <c r="E208" s="14"/>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A209" s="14" t="s">
         <v>113</v>
       </c>
@@ -7551,7 +7566,7 @@
       </c>
       <c r="E209" s="14"/>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A210" s="14" t="s">
         <v>113</v>
       </c>
@@ -7566,7 +7581,7 @@
       </c>
       <c r="E210" s="14"/>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A211" s="14" t="s">
         <v>113</v>
       </c>
@@ -7581,7 +7596,7 @@
       </c>
       <c r="E211" s="14"/>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A212" s="14" t="s">
         <v>113</v>
       </c>
@@ -7596,7 +7611,7 @@
       </c>
       <c r="E212" s="14"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A213" s="14" t="s">
         <v>113</v>
       </c>
@@ -7611,7 +7626,7 @@
       </c>
       <c r="E213" s="14"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A214" s="14" t="s">
         <v>113</v>
       </c>
@@ -7626,7 +7641,7 @@
       </c>
       <c r="E214" s="14"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A215" s="14" t="s">
         <v>113</v>
       </c>
@@ -7641,7 +7656,7 @@
       </c>
       <c r="E215" s="14"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A216" s="14" t="s">
         <v>113</v>
       </c>
@@ -7656,7 +7671,7 @@
       </c>
       <c r="E216" s="14"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A217" s="14" t="s">
         <v>113</v>
       </c>
@@ -7671,7 +7686,7 @@
       </c>
       <c r="E217" s="14"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A218" s="14" t="s">
         <v>113</v>
       </c>
@@ -7686,7 +7701,7 @@
       </c>
       <c r="E218" s="14"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A219" s="14" t="s">
         <v>113</v>
       </c>
@@ -7701,7 +7716,7 @@
       </c>
       <c r="E219" s="14"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A220" s="14" t="s">
         <v>113</v>
       </c>
@@ -7716,7 +7731,7 @@
       </c>
       <c r="E220" s="14"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A221" s="14" t="s">
         <v>113</v>
       </c>
@@ -7731,7 +7746,7 @@
       </c>
       <c r="E221" s="14"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A222" s="14" t="s">
         <v>113</v>
       </c>
@@ -7746,7 +7761,7 @@
       </c>
       <c r="E222" s="14"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A223" s="14" t="s">
         <v>113</v>
       </c>
@@ -7761,7 +7776,7 @@
       </c>
       <c r="E223" s="14"/>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A224" s="14" t="s">
         <v>113</v>
       </c>
@@ -7776,7 +7791,7 @@
       </c>
       <c r="E224" s="14"/>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A225" s="14" t="s">
         <v>113</v>
       </c>
@@ -7791,7 +7806,7 @@
       </c>
       <c r="E225" s="14"/>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A226" s="14" t="s">
         <v>113</v>
       </c>
@@ -7806,7 +7821,7 @@
       </c>
       <c r="E226" s="14"/>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A227" s="14" t="s">
         <v>113</v>
       </c>
@@ -7821,7 +7836,7 @@
       </c>
       <c r="E227" s="14"/>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A228" s="14" t="s">
         <v>113</v>
       </c>
@@ -7836,7 +7851,7 @@
       </c>
       <c r="E228" s="14"/>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A229" s="14" t="s">
         <v>113</v>
       </c>
@@ -7851,7 +7866,7 @@
       </c>
       <c r="E229" s="14"/>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A230" s="14" t="s">
         <v>113</v>
       </c>
@@ -7866,7 +7881,7 @@
       </c>
       <c r="E230" s="14"/>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A231" s="14" t="s">
         <v>113</v>
       </c>
@@ -7881,7 +7896,7 @@
       </c>
       <c r="E231" s="14"/>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A232" s="14" t="s">
         <v>113</v>
       </c>
@@ -7896,7 +7911,7 @@
       </c>
       <c r="E232" s="14"/>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A233" s="14" t="s">
         <v>113</v>
       </c>
@@ -7911,7 +7926,7 @@
       </c>
       <c r="E233" s="14"/>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A234" s="14" t="s">
         <v>113</v>
       </c>
@@ -7926,7 +7941,7 @@
       </c>
       <c r="E234" s="14"/>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A235" s="14" t="s">
         <v>113</v>
       </c>
@@ -7941,7 +7956,7 @@
       </c>
       <c r="E235" s="14"/>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A236" s="14" t="s">
         <v>113</v>
       </c>
@@ -7956,7 +7971,7 @@
       </c>
       <c r="E236" s="14"/>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A237" s="14" t="s">
         <v>113</v>
       </c>
@@ -7971,7 +7986,7 @@
       </c>
       <c r="E237" s="14"/>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A238" s="14" t="s">
         <v>113</v>
       </c>
@@ -7986,7 +8001,7 @@
       </c>
       <c r="E238" s="14"/>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A239" s="14" t="s">
         <v>113</v>
       </c>
@@ -8001,7 +8016,7 @@
       </c>
       <c r="E239" s="14"/>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A240" s="14" t="s">
         <v>113</v>
       </c>
@@ -8016,7 +8031,7 @@
       </c>
       <c r="E240" s="14"/>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A241" s="14" t="s">
         <v>113</v>
       </c>
@@ -8031,12 +8046,12 @@
       </c>
       <c r="E241" s="14"/>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.5">
       <c r="C242" s="14"/>
       <c r="D242" s="14"/>
       <c r="E242" s="14"/>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A243" s="14" t="s">
         <v>114</v>
       </c>
@@ -8051,7 +8066,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A244" s="14" t="s">
         <v>114</v>
       </c>
@@ -8066,7 +8081,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A245" s="14" t="s">
         <v>114</v>
       </c>
@@ -8081,7 +8096,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A246" s="14" t="s">
         <v>114</v>
       </c>
@@ -8096,7 +8111,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A247" s="14" t="s">
         <v>114</v>
       </c>
@@ -8111,7 +8126,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A248" s="14" t="s">
         <v>114</v>
       </c>
@@ -8126,7 +8141,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A249" s="14" t="s">
         <v>114</v>
       </c>
@@ -8141,7 +8156,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A250" s="14" t="s">
         <v>114</v>
       </c>
@@ -8156,7 +8171,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A251" s="14" t="s">
         <v>114</v>
       </c>
@@ -8171,7 +8186,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A252" s="14" t="s">
         <v>114</v>
       </c>
@@ -8186,7 +8201,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A253" s="14" t="s">
         <v>114</v>
       </c>
@@ -8201,7 +8216,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A254" s="14" t="s">
         <v>114</v>
       </c>
@@ -8216,7 +8231,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A255" s="14" t="s">
         <v>114</v>
       </c>
@@ -8231,7 +8246,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A256" s="14" t="s">
         <v>114</v>
       </c>
@@ -8246,7 +8261,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A257" s="14" t="s">
         <v>114</v>
       </c>
@@ -8261,7 +8276,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A258" s="14" t="s">
         <v>114</v>
       </c>
@@ -8276,7 +8291,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A259" s="14" t="s">
         <v>114</v>
       </c>
@@ -8291,7 +8306,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A260" s="14" t="s">
         <v>114</v>
       </c>
@@ -8306,7 +8321,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A261" s="14" t="s">
         <v>114</v>
       </c>
@@ -8321,7 +8336,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A262" s="14" t="s">
         <v>114</v>
       </c>
@@ -8336,7 +8351,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A263" s="14" t="s">
         <v>114</v>
       </c>
@@ -8351,7 +8366,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A264" s="14" t="s">
         <v>114</v>
       </c>
@@ -8366,7 +8381,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A265" s="14" t="s">
         <v>114</v>
       </c>
@@ -8381,7 +8396,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A266" s="14" t="s">
         <v>114</v>
       </c>
@@ -8396,7 +8411,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A267" s="14" t="s">
         <v>114</v>
       </c>
@@ -8411,7 +8426,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A268" s="14" t="s">
         <v>114</v>
       </c>
@@ -8426,7 +8441,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A269" s="14" t="s">
         <v>114</v>
       </c>
@@ -8441,7 +8456,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A270" s="14" t="s">
         <v>114</v>
       </c>
@@ -8456,7 +8471,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A271" s="14" t="s">
         <v>114</v>
       </c>
@@ -8471,7 +8486,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A272" s="14" t="s">
         <v>114</v>
       </c>
@@ -8486,7 +8501,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A273" s="14" t="s">
         <v>114</v>
       </c>
@@ -8501,7 +8516,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A274" s="14" t="s">
         <v>114</v>
       </c>
@@ -8516,7 +8531,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A275" s="14" t="s">
         <v>114</v>
       </c>
@@ -8531,7 +8546,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A276" s="14" t="s">
         <v>114</v>
       </c>
@@ -8546,7 +8561,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A277" s="14" t="s">
         <v>114</v>
       </c>
@@ -8561,7 +8576,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A278" s="14" t="s">
         <v>114</v>
       </c>
@@ -8576,7 +8591,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A279" s="14" t="s">
         <v>114</v>
       </c>
@@ -8591,7 +8606,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A280" s="14" t="s">
         <v>114</v>
       </c>
@@ -8606,7 +8621,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A281" s="14" t="s">
         <v>114</v>
       </c>
@@ -8621,7 +8636,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A282" s="14" t="s">
         <v>114</v>
       </c>
@@ -8636,7 +8651,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A283" s="14" t="s">
         <v>114</v>
       </c>
@@ -8651,7 +8666,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A284" s="14" t="s">
         <v>114</v>
       </c>
@@ -8666,7 +8681,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A285" s="14" t="s">
         <v>114</v>
       </c>
@@ -8681,7 +8696,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A286" s="14" t="s">
         <v>114</v>
       </c>
@@ -8696,7 +8711,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A287" s="14" t="s">
         <v>114</v>
       </c>
@@ -8711,7 +8726,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A288" s="14" t="s">
         <v>114</v>
       </c>
@@ -8726,7 +8741,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A289" s="14" t="s">
         <v>114</v>
       </c>
@@ -8741,7 +8756,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A290" s="14" t="s">
         <v>114</v>
       </c>
@@ -8756,7 +8771,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A291" s="14" t="s">
         <v>114</v>
       </c>
@@ -8771,7 +8786,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A292" s="14" t="s">
         <v>114</v>
       </c>
@@ -8786,7 +8801,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A293" s="14" t="s">
         <v>114</v>
       </c>
@@ -8801,7 +8816,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A294" s="14" t="s">
         <v>114</v>
       </c>
@@ -8816,7 +8831,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A295" s="14" t="s">
         <v>114</v>
       </c>
@@ -8831,7 +8846,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A296" s="14" t="s">
         <v>114</v>
       </c>
@@ -8846,7 +8861,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A297" s="14" t="s">
         <v>114</v>
       </c>
@@ -8861,7 +8876,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A298" s="14" t="s">
         <v>114</v>
       </c>
@@ -8876,7 +8891,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A299" s="14" t="s">
         <v>114</v>
       </c>
@@ -8891,7 +8906,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A300" s="14" t="s">
         <v>114</v>
       </c>
@@ -8906,7 +8921,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A301" s="14" t="s">
         <v>114</v>
       </c>
@@ -8921,7 +8936,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A302" s="14" t="s">
         <v>114</v>
       </c>
@@ -8936,7 +8951,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A303" s="14" t="s">
         <v>114</v>
       </c>
@@ -8951,7 +8966,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A304" s="14" t="s">
         <v>114</v>
       </c>
@@ -8966,7 +8981,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A305" s="14" t="s">
         <v>114</v>
       </c>
@@ -8981,7 +8996,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A306" s="14" t="s">
         <v>114</v>
       </c>
@@ -8996,7 +9011,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A307" s="14" t="s">
         <v>114</v>
       </c>
@@ -9011,7 +9026,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A308" s="14" t="s">
         <v>114</v>
       </c>
@@ -9026,7 +9041,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A309" s="14" t="s">
         <v>114</v>
       </c>
@@ -9041,7 +9056,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A310" s="14" t="s">
         <v>114</v>
       </c>
@@ -9056,7 +9071,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A311" s="14" t="s">
         <v>114</v>
       </c>
@@ -9071,7 +9086,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A312" s="14" t="s">
         <v>114</v>
       </c>
@@ -9086,7 +9101,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A313" s="14" t="s">
         <v>114</v>
       </c>
@@ -9101,7 +9116,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A314" s="14" t="s">
         <v>114</v>
       </c>
@@ -9116,7 +9131,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A315" s="14" t="s">
         <v>114</v>
       </c>
@@ -9131,7 +9146,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A316" s="14" t="s">
         <v>114</v>
       </c>
@@ -9146,7 +9161,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A317" s="14" t="s">
         <v>114</v>
       </c>
@@ -9161,7 +9176,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A318" s="14" t="s">
         <v>114</v>
       </c>
@@ -9176,7 +9191,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A319" s="14" t="s">
         <v>114</v>
       </c>
@@ -9191,7 +9206,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A320" s="14" t="s">
         <v>114</v>
       </c>
@@ -9206,7 +9221,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A321" s="14" t="s">
         <v>114</v>
       </c>
@@ -9221,7 +9236,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A322" s="14" t="s">
         <v>114</v>
       </c>
@@ -9236,7 +9251,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A323" s="14" t="s">
         <v>114</v>
       </c>
@@ -9251,7 +9266,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A324" s="14" t="s">
         <v>114</v>
       </c>
@@ -9266,7 +9281,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A325" s="14" t="s">
         <v>114</v>
       </c>
@@ -9281,7 +9296,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A326" s="14" t="s">
         <v>114</v>
       </c>
@@ -9296,7 +9311,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A327" s="14" t="s">
         <v>114</v>
       </c>
@@ -9311,7 +9326,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A328" s="14" t="s">
         <v>114</v>
       </c>
@@ -9326,7 +9341,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A329" s="14" t="s">
         <v>114</v>
       </c>
@@ -9341,7 +9356,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A330" s="14" t="s">
         <v>114</v>
       </c>
@@ -9356,7 +9371,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A331" s="14" t="s">
         <v>114</v>
       </c>
@@ -9371,7 +9386,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A332" s="14" t="s">
         <v>114</v>
       </c>
@@ -9386,7 +9401,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A333" s="14" t="s">
         <v>114</v>
       </c>
@@ -9401,7 +9416,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A334" s="14" t="s">
         <v>114</v>
       </c>
@@ -9416,7 +9431,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A335" s="14" t="s">
         <v>114</v>
       </c>
@@ -9431,7 +9446,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A336" s="14" t="s">
         <v>114</v>
       </c>
@@ -9446,7 +9461,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A337" s="14" t="s">
         <v>114</v>
       </c>
@@ -9461,7 +9476,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A338" s="14" t="s">
         <v>114</v>
       </c>
@@ -9476,7 +9491,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A339" s="14" t="s">
         <v>114</v>
       </c>
@@ -9491,7 +9506,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A340" s="14" t="s">
         <v>114</v>
       </c>
@@ -9506,7 +9521,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A341" s="14" t="s">
         <v>114</v>
       </c>
@@ -9521,7 +9536,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A342" s="14" t="s">
         <v>114</v>
       </c>
@@ -9536,7 +9551,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A343" s="14" t="s">
         <v>114</v>
       </c>
@@ -9551,7 +9566,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A344" s="14" t="s">
         <v>114</v>
       </c>
@@ -9566,7 +9581,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A345" s="14" t="s">
         <v>114</v>
       </c>
@@ -9581,7 +9596,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A346" s="14" t="s">
         <v>114</v>
       </c>
@@ -9596,7 +9611,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A347" s="14" t="s">
         <v>114</v>
       </c>
@@ -9611,7 +9626,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A348" s="14" t="s">
         <v>114</v>
       </c>
@@ -9626,7 +9641,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A349" s="14" t="s">
         <v>114</v>
       </c>
@@ -9641,7 +9656,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A350" s="14" t="s">
         <v>114</v>
       </c>
@@ -9656,7 +9671,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A351" s="14" t="s">
         <v>114</v>
       </c>
@@ -9671,7 +9686,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A352" s="14" t="s">
         <v>114</v>
       </c>
@@ -9686,7 +9701,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A353" s="14" t="s">
         <v>114</v>
       </c>
@@ -9701,7 +9716,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A354" s="14" t="s">
         <v>114</v>
       </c>
@@ -9716,7 +9731,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A355" s="14" t="s">
         <v>114</v>
       </c>
@@ -9731,7 +9746,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A356" s="14" t="s">
         <v>114</v>
       </c>
@@ -9746,7 +9761,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A357" s="14" t="s">
         <v>114</v>
       </c>
@@ -9761,7 +9776,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A358" s="14" t="s">
         <v>114</v>
       </c>
@@ -9776,7 +9791,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A359" s="14" t="s">
         <v>114</v>
       </c>
@@ -9791,7 +9806,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A360" s="14" t="s">
         <v>114</v>
       </c>
@@ -9806,7 +9821,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A361" s="14" t="s">
         <v>114</v>
       </c>
@@ -9821,7 +9836,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A362" s="14" t="s">
         <v>114</v>
       </c>
@@ -9836,7 +9851,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A363" s="14" t="s">
         <v>114</v>
       </c>
@@ -9851,7 +9866,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A364" s="14" t="s">
         <v>114</v>
       </c>
@@ -9866,7 +9881,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A365" s="14" t="s">
         <v>114</v>
       </c>
@@ -9881,7 +9896,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A366" s="14" t="s">
         <v>114</v>
       </c>
@@ -9896,7 +9911,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A367" s="14" t="s">
         <v>114</v>
       </c>
@@ -9911,7 +9926,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A368" s="14" t="s">
         <v>114</v>
       </c>
@@ -9926,7 +9941,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A369" s="14" t="s">
         <v>114</v>
       </c>
@@ -9941,7 +9956,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A370" s="14" t="s">
         <v>114</v>
       </c>
@@ -9956,7 +9971,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A371" s="14" t="s">
         <v>114</v>
       </c>
@@ -9971,7 +9986,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A372" s="14" t="s">
         <v>114</v>
       </c>
@@ -9986,7 +10001,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A373" s="14" t="s">
         <v>114</v>
       </c>
@@ -10001,7 +10016,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A374" s="14" t="s">
         <v>114</v>
       </c>
@@ -10016,7 +10031,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A375" s="14" t="s">
         <v>114</v>
       </c>
@@ -10031,7 +10046,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A376" s="14" t="s">
         <v>114</v>
       </c>
@@ -10046,7 +10061,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A377" s="14" t="s">
         <v>114</v>
       </c>
@@ -10061,7 +10076,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A378" s="14" t="s">
         <v>114</v>
       </c>
@@ -10076,7 +10091,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A379" s="14" t="s">
         <v>114</v>
       </c>
@@ -10091,7 +10106,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A380" s="14" t="s">
         <v>114</v>
       </c>
@@ -10106,7 +10121,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A381" s="14" t="s">
         <v>114</v>
       </c>
@@ -10121,7 +10136,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A382" s="14" t="s">
         <v>114</v>
       </c>
@@ -10136,7 +10151,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A383" s="14" t="s">
         <v>114</v>
       </c>
@@ -10151,7 +10166,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A384" s="14" t="s">
         <v>114</v>
       </c>
@@ -10166,7 +10181,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A385" s="14" t="s">
         <v>114</v>
       </c>
@@ -10181,7 +10196,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A386" s="14" t="s">
         <v>114</v>
       </c>
@@ -10196,7 +10211,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A387" s="14" t="s">
         <v>114</v>
       </c>
@@ -10211,7 +10226,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A388" s="14" t="s">
         <v>114</v>
       </c>
@@ -10226,7 +10241,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A389" s="14" t="s">
         <v>114</v>
       </c>
@@ -10241,7 +10256,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A390" s="14" t="s">
         <v>114</v>
       </c>
@@ -10256,7 +10271,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A391" s="14" t="s">
         <v>114</v>
       </c>
@@ -10271,7 +10286,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A392" s="14" t="s">
         <v>114</v>
       </c>
@@ -10286,7 +10301,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A393" s="14" t="s">
         <v>114</v>
       </c>
@@ -10301,7 +10316,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A394" s="14" t="s">
         <v>114</v>
       </c>
@@ -10316,7 +10331,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A395" s="14" t="s">
         <v>114</v>
       </c>
@@ -10331,7 +10346,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A396" s="14" t="s">
         <v>114</v>
       </c>
@@ -10346,7 +10361,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A397" s="14" t="s">
         <v>114</v>
       </c>
@@ -10361,7 +10376,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A398" s="14" t="s">
         <v>114</v>
       </c>
@@ -10376,7 +10391,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A399" s="14" t="s">
         <v>114</v>
       </c>
@@ -10391,7 +10406,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A400" s="14" t="s">
         <v>114</v>
       </c>
@@ -10406,7 +10421,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A401" s="14" t="s">
         <v>114</v>
       </c>
@@ -10421,7 +10436,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A402" s="14" t="s">
         <v>114</v>
       </c>
@@ -10436,7 +10451,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A403" s="14" t="s">
         <v>114</v>
       </c>
@@ -10451,7 +10466,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A404" s="14" t="s">
         <v>114</v>
       </c>
@@ -10466,7 +10481,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A405" s="14" t="s">
         <v>114</v>
       </c>
@@ -10481,7 +10496,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A406" s="14" t="s">
         <v>114</v>
       </c>
@@ -10496,7 +10511,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A407" s="14" t="s">
         <v>114</v>
       </c>
@@ -10511,7 +10526,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A408" s="14" t="s">
         <v>114</v>
       </c>
@@ -10526,7 +10541,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A409" s="14" t="s">
         <v>114</v>
       </c>
@@ -10541,7 +10556,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A410" s="14" t="s">
         <v>114</v>
       </c>
@@ -10556,7 +10571,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A411" s="14" t="s">
         <v>114</v>
       </c>
@@ -10571,7 +10586,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A412" s="40" t="s">
         <v>114</v>
       </c>
@@ -10586,7 +10601,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A413" s="14" t="s">
         <v>114</v>
       </c>
@@ -10601,7 +10616,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A414" s="14" t="s">
         <v>114</v>
       </c>
@@ -10616,7 +10631,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A415" s="14" t="s">
         <v>114</v>
       </c>
@@ -10631,7 +10646,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A416" s="14" t="s">
         <v>114</v>
       </c>
@@ -10646,7 +10661,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A417" s="14" t="s">
         <v>114</v>
       </c>
@@ -10661,7 +10676,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A418" s="14" t="s">
         <v>114</v>
       </c>
@@ -10676,7 +10691,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A419" s="14" t="s">
         <v>114</v>
       </c>
@@ -10691,7 +10706,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A420" s="14" t="s">
         <v>114</v>
       </c>
@@ -10706,7 +10721,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A421" s="14" t="s">
         <v>114</v>
       </c>
@@ -10721,7 +10736,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A422" s="14" t="s">
         <v>114</v>
       </c>
@@ -10736,7 +10751,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A423" s="14" t="s">
         <v>114</v>
       </c>
@@ -10751,7 +10766,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A424" s="14" t="s">
         <v>114</v>
       </c>
@@ -10766,7 +10781,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A425" s="14" t="s">
         <v>114</v>
       </c>
@@ -10781,7 +10796,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A426" s="14" t="s">
         <v>114</v>
       </c>
@@ -10796,7 +10811,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A427" s="14" t="s">
         <v>114</v>
       </c>
@@ -10811,7 +10826,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A428" s="14" t="s">
         <v>114</v>
       </c>
@@ -10826,7 +10841,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A429" s="14" t="s">
         <v>114</v>
       </c>
@@ -10841,7 +10856,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A430" s="14" t="s">
         <v>114</v>
       </c>
@@ -10856,7 +10871,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A431" s="14" t="s">
         <v>114</v>
       </c>
@@ -10871,7 +10886,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A432" s="14" t="s">
         <v>114</v>
       </c>
@@ -10886,7 +10901,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A433" s="14" t="s">
         <v>114</v>
       </c>
@@ -10901,7 +10916,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A434" s="14" t="s">
         <v>114</v>
       </c>
@@ -10916,7 +10931,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A435" s="14" t="s">
         <v>114</v>
       </c>
@@ -10931,7 +10946,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A436" s="14" t="s">
         <v>114</v>
       </c>
@@ -10946,7 +10961,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A437" s="14" t="s">
         <v>114</v>
       </c>
@@ -10961,7 +10976,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A438" s="14" t="s">
         <v>114</v>
       </c>
@@ -10976,7 +10991,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A439" s="14" t="s">
         <v>114</v>
       </c>
@@ -10991,7 +11006,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A440" s="14" t="s">
         <v>114</v>
       </c>
@@ -11006,7 +11021,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A441" s="14" t="s">
         <v>114</v>
       </c>
@@ -11021,7 +11036,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A442" s="14" t="s">
         <v>114</v>
       </c>
@@ -11036,7 +11051,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A443" s="14" t="s">
         <v>114</v>
       </c>
@@ -11051,7 +11066,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A444" s="14" t="s">
         <v>114</v>
       </c>
@@ -11066,7 +11081,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A445" s="14" t="s">
         <v>114</v>
       </c>
@@ -11081,7 +11096,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A446" s="14" t="s">
         <v>114</v>
       </c>
@@ -11096,7 +11111,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="447" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A447" s="14" t="s">
         <v>114</v>
       </c>
@@ -11111,7 +11126,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="448" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A448" s="14" t="s">
         <v>114</v>
       </c>
@@ -11126,7 +11141,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="449" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A449" s="14" t="s">
         <v>114</v>
       </c>
@@ -11141,7 +11156,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="450" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A450" s="14" t="s">
         <v>114</v>
       </c>
@@ -11169,18 +11184,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.41015625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.41015625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="30" t="s">
         <v>330</v>
       </c>
@@ -11194,15 +11209,15 @@
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>703</v>
+        <v>712</v>
       </c>
       <c r="B2" t="s">
-        <v>705</v>
-      </c>
-      <c r="C2">
-        <v>202105</v>
+        <v>710</v>
+      </c>
+      <c r="C2" t="s">
+        <v>711</v>
       </c>
       <c r="D2" t="s">
         <v>334</v>

</xml_diff>